<commit_message>
added search string + criteria
</commit_message>
<xml_diff>
--- a/src/analysis.xlsx
+++ b/src/analysis.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rim\Desktop\SPLC22_paper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rim\Documents\GitHub\SecurityConfigurableStorage_SPLC22\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,12 +15,11 @@
     <sheet name="analysis" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="132">
   <si>
     <t>title</t>
   </si>
@@ -410,6 +409,12 @@
   </si>
   <si>
     <t>Dimitri Van Landuyt, Stefan Walraven,  Wouter Joosen</t>
+  </si>
+  <si>
+    <t>("software as a service" OR "SaaS" OR "infrastructure as a service" OR "IaaS" OR "service-based" OR "service-oriented" OR "on-demand" OR "stor*" OR "cloud" OR "database" OR "warehouse" OR "blockchain" OR "edge" OR "fog") AND ("software product line" OR "SPL" OR "product famil*" OR "system famil*" OR “software famil*” OR "variant*rich" OR "config* system") AND ("security" OR "secure")</t>
+  </si>
+  <si>
+    <t>String</t>
   </si>
 </sst>
 </file>
@@ -1219,10 +1224,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X54"/>
+  <dimension ref="A1:X58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.85" x14ac:dyDescent="0.25"/>
@@ -2058,6 +2063,16 @@
         <v>2021</v>
       </c>
     </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>130</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>